<commit_message>
changes made through the internship roadmap
</commit_message>
<xml_diff>
--- a/All Documents/Internship Work Flow/HPL Internship Daily Tasks.xlsx
+++ b/All Documents/Internship Work Flow/HPL Internship Daily Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship\SQA-Internship-Progress-in-HPL\All Documents\Internship Work Flow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F88ECF7-5A11-4625-A898-991B81D54758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6818E5-8EF2-41A1-872F-806C46557600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -317,6 +317,61 @@
     <t xml:space="preserve">1. Created test cases for Pulse App Sri Lanka
 2. Manually tested features: Doctor Management, DCR, Tour Plan, Check In / Check Out, Geofence
 3. Called zonal heads regarding MOF Entry </t>
+  </si>
+  <si>
+    <t>1. Mailed test documents(Test Execution Report, Defect Report) to Team
+2. Mailed MOF Entry Remarks to Khaled Sir
+3. Got new task to test SAP Modules - Assigned by Khaled Sir
+4. Started exploring Jira - Zephyr</t>
+  </si>
+  <si>
+    <t>1. Exploring Jira - Zephyr (Imported Manual Test Cases into Zephyr)
+2. Worked on JS Tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Worked on JS Tasks
+2. Worked on Zephyr
+3. Khaled Sir will provide update on SAP </t>
+  </si>
+  <si>
+    <t>1. Worked on JS Tasks
+2. Tested SAP - Product Allocation Module
+3. New Assignment - Shahiduzzaman Sir - HCL Website - Deadline - 15-10-25</t>
+  </si>
+  <si>
+    <t>1. Worked on HCL Website Assignment</t>
+  </si>
+  <si>
+    <t>1. HCL Website Assignment
+2. Completed SAP - Product Allocation Module Test
+3. Completed Phase - 1 of Roadmap.(Completing Watching JS Videos - 90+ Completed) (Not Submitted to Anik Vaiya Yet.)</t>
+  </si>
+  <si>
+    <t>1. Working on HCL Website
+2. Starting Phase - 2 of the Roadmap</t>
+  </si>
+  <si>
+    <t>1. HCL Website Assignment
+2. Started Phase - 2 of the Roadmap</t>
+  </si>
+  <si>
+    <t>1. HCL Website Update - 
+(About Us , Mission &amp; Vission , Meet Our Leaders)
+2. Talked with Nayeem Vai - First make demo, then resources will be given. 
+Take References from HPL , bdhfl</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>1. HCL Website Update - 
+(About Us , Mission &amp; Vission , Meet Our Leaders)</t>
+  </si>
+  <si>
+    <t>VACATION</t>
   </si>
 </sst>
 </file>
@@ -740,8 +795,8 @@
   </sheetPr>
   <dimension ref="A1:J182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="51" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110:C112"/>
+    <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,10 +2386,16 @@
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
     </row>
-    <row r="106" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" s="3"/>
-      <c r="B106" s="3"/>
-      <c r="C106" s="4"/>
+    <row r="106" spans="1:10" ht="211.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="2">
+        <v>45915</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
       <c r="F106" s="7"/>
@@ -2343,10 +2404,16 @@
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
     </row>
-    <row r="107" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="3"/>
-      <c r="B107" s="3"/>
-      <c r="C107" s="4"/>
+    <row r="107" spans="1:10" ht="105.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="2">
+        <v>45916</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
       <c r="F107" s="7"/>
@@ -2355,10 +2422,16 @@
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
     </row>
-    <row r="108" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108" s="3"/>
-      <c r="B108" s="3"/>
-      <c r="C108" s="4"/>
+    <row r="108" spans="1:10" ht="114.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="2">
+        <v>45917</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
       <c r="F108" s="7"/>
@@ -2367,10 +2440,16 @@
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
     </row>
-    <row r="109" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="3"/>
-      <c r="B109" s="3"/>
-      <c r="C109" s="4"/>
+    <row r="109" spans="1:10" ht="171" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="2">
+        <v>45918</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
@@ -2380,9 +2459,15 @@
       <c r="J109" s="7"/>
     </row>
     <row r="110" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="3"/>
-      <c r="B110" s="3"/>
-      <c r="C110" s="4"/>
+      <c r="A110" s="2">
+        <v>45921</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
       <c r="F110" s="7"/>
@@ -2391,10 +2476,16 @@
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
     </row>
-    <row r="111" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="3"/>
-      <c r="B111" s="3"/>
-      <c r="C111" s="4"/>
+    <row r="111" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="2">
+        <v>45922</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
       <c r="F111" s="7"/>
@@ -2403,10 +2494,16 @@
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
     </row>
-    <row r="112" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A112" s="3"/>
-      <c r="B112" s="3"/>
-      <c r="C112" s="4"/>
+    <row r="112" spans="1:10" ht="70.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" s="2">
+        <v>45923</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
       <c r="F112" s="7"/>
@@ -2416,9 +2513,15 @@
       <c r="J112" s="7"/>
     </row>
     <row r="113" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="3"/>
-      <c r="B113" s="3"/>
-      <c r="C113" s="4"/>
+      <c r="A113" s="2">
+        <v>45924</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
       <c r="F113" s="7"/>
@@ -2428,9 +2531,15 @@
       <c r="J113" s="7"/>
     </row>
     <row r="114" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" s="3"/>
-      <c r="B114" s="3"/>
-      <c r="C114" s="4"/>
+      <c r="A114" s="2">
+        <v>45925</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="D114" s="7"/>
       <c r="E114" s="7"/>
       <c r="F114" s="7"/>
@@ -2439,10 +2548,16 @@
       <c r="I114" s="7"/>
       <c r="J114" s="7"/>
     </row>
-    <row r="115" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="3"/>
-      <c r="B115" s="3"/>
-      <c r="C115" s="4"/>
+    <row r="115" spans="1:10" ht="70.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="2">
+        <v>45928</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
       <c r="F115" s="7"/>
@@ -2451,10 +2566,16 @@
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
     </row>
-    <row r="116" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" s="3"/>
-      <c r="B116" s="3"/>
-      <c r="C116" s="4"/>
+    <row r="116" spans="1:10" ht="176.25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="2">
+        <v>45929</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
       <c r="F116" s="7"/>
@@ -2463,10 +2584,16 @@
       <c r="I116" s="7"/>
       <c r="J116" s="7"/>
     </row>
-    <row r="117" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="3"/>
-      <c r="B117" s="3"/>
-      <c r="C117" s="4"/>
+    <row r="117" spans="1:10" ht="70.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="2">
+        <v>45930</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
       <c r="F117" s="7"/>
@@ -2476,9 +2603,15 @@
       <c r="J117" s="7"/>
     </row>
     <row r="118" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="4"/>
+      <c r="A118" s="2">
+        <v>45931</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="D118" s="7"/>
       <c r="E118" s="7"/>
       <c r="F118" s="7"/>
@@ -2488,9 +2621,15 @@
       <c r="J118" s="7"/>
     </row>
     <row r="119" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
-      <c r="C119" s="4"/>
+      <c r="A119" s="2">
+        <v>45932</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="D119" s="7"/>
       <c r="E119" s="7"/>
       <c r="F119" s="7"/>
@@ -2500,9 +2639,15 @@
       <c r="J119" s="7"/>
     </row>
     <row r="120" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="4"/>
+      <c r="A120" s="2">
+        <v>45933</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="D120" s="7"/>
       <c r="E120" s="7"/>
       <c r="F120" s="7"/>
@@ -2512,9 +2657,15 @@
       <c r="J120" s="7"/>
     </row>
     <row r="121" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="7"/>
-      <c r="B121" s="7"/>
-      <c r="C121" s="4"/>
+      <c r="A121" s="2">
+        <v>45934</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
       <c r="F121" s="7"/>
@@ -2524,8 +2675,12 @@
       <c r="J121" s="7"/>
     </row>
     <row r="122" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" s="7"/>
-      <c r="B122" s="7"/>
+      <c r="A122" s="2">
+        <v>45935</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="7"/>
@@ -2536,8 +2691,12 @@
       <c r="J122" s="7"/>
     </row>
     <row r="123" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A123" s="7"/>
-      <c r="B123" s="7"/>
+      <c r="A123" s="2">
+        <v>45936</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="7"/>
@@ -2548,8 +2707,12 @@
       <c r="J123" s="7"/>
     </row>
     <row r="124" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="7"/>
-      <c r="B124" s="7"/>
+      <c r="A124" s="2">
+        <v>45937</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="7"/>
@@ -2560,8 +2723,12 @@
       <c r="J124" s="7"/>
     </row>
     <row r="125" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" s="7"/>
-      <c r="B125" s="7"/>
+      <c r="A125" s="2">
+        <v>45938</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="7"/>
@@ -2572,8 +2739,12 @@
       <c r="J125" s="7"/>
     </row>
     <row r="126" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A126" s="7"/>
-      <c r="B126" s="7"/>
+      <c r="A126" s="2">
+        <v>45939</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
@@ -2585,7 +2756,7 @@
     </row>
     <row r="127" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="7"/>
-      <c r="B127" s="7"/>
+      <c r="B127" s="3"/>
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="7"/>
@@ -2597,7 +2768,7 @@
     </row>
     <row r="128" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="7"/>
-      <c r="B128" s="7"/>
+      <c r="B128" s="3"/>
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="7"/>

</xml_diff>